<commit_message>
Make MAIR plots (parity, histogram)
</commit_message>
<xml_diff>
--- a/02_meter_data/summary_files/MAIR.xlsx
+++ b/02_meter_data/summary_files/MAIR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/02_meter_data/summary_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06C82C6-8CE1-8743-A534-789ECC0A5597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821962F5-82E3-6C43-B2A1-46546CA55570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36320" yWindow="500" windowWidth="34560" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -658,6 +658,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -782,9 +785,6 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
         <v>0</v>
       </c>
@@ -863,7 +863,7 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -943,7 +943,7 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1023,7 +1023,7 @@
         <v>4</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1103,7 +1103,7 @@
         <v>5</v>
       </c>
       <c r="G6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1183,7 +1183,7 @@
         <v>6</v>
       </c>
       <c r="G7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1263,7 +1263,7 @@
         <v>7</v>
       </c>
       <c r="G8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1343,7 +1343,7 @@
         <v>8</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1423,7 +1423,7 @@
         <v>9</v>
       </c>
       <c r="G10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1502,9 +1502,6 @@
       <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11">
-        <v>10</v>
-      </c>
       <c r="H11">
         <v>0</v>
       </c>
@@ -1583,7 +1580,7 @@
         <v>11</v>
       </c>
       <c r="G12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1663,7 +1660,7 @@
         <v>12</v>
       </c>
       <c r="G13">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1743,7 +1740,7 @@
         <v>13</v>
       </c>
       <c r="G14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1823,7 +1820,7 @@
         <v>14</v>
       </c>
       <c r="G15">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1903,7 +1900,7 @@
         <v>15</v>
       </c>
       <c r="G16">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1983,7 +1980,7 @@
         <v>16</v>
       </c>
       <c r="G17">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2063,7 +2060,7 @@
         <v>17</v>
       </c>
       <c r="G18">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -2143,7 +2140,7 @@
         <v>18</v>
       </c>
       <c r="G19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2223,7 +2220,7 @@
         <v>19</v>
       </c>
       <c r="G20">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -2303,7 +2300,7 @@
         <v>20</v>
       </c>
       <c r="G21">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -2383,7 +2380,7 @@
         <v>21</v>
       </c>
       <c r="G22">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -2463,7 +2460,7 @@
         <v>22</v>
       </c>
       <c r="G23">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2543,7 +2540,7 @@
         <v>23</v>
       </c>
       <c r="G24">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -2623,7 +2620,7 @@
         <v>24</v>
       </c>
       <c r="G25">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -2703,7 +2700,7 @@
         <v>25</v>
       </c>
       <c r="G26">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -2783,7 +2780,7 @@
         <v>26</v>
       </c>
       <c r="G27">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H27">
         <v>0</v>

</xml_diff>

<commit_message>
Run QC analysis on Carbon Mapper and Kairos
</commit_message>
<xml_diff>
--- a/02_meter_data/summary_files/MAIR.xlsx
+++ b/02_meter_data/summary_files/MAIR.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/02_meter_data/summary_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippineburdeau/Desktop/Stanford/Methane group/Controlled Releases/Analysis - airplanes/Summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821962F5-82E3-6C43-B2A1-46546CA55570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C041A99A-AA06-5347-956E-54089DFB0C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36320" yWindow="500" windowWidth="34560" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1080" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="112">
   <si>
     <t>Date</t>
   </si>
@@ -139,6 +139,9 @@
     <t>17:15:06</t>
   </si>
   <si>
+    <t>17:15:00</t>
+  </si>
+  <si>
     <t>Mama Coriolis</t>
   </si>
   <si>
@@ -148,12 +151,18 @@
     <t>17:32:51</t>
   </si>
   <si>
+    <t>17:32:00</t>
+  </si>
+  <si>
     <t>17:50:42</t>
   </si>
   <si>
     <t>17:50:38</t>
   </si>
   <si>
+    <t>17:51:00</t>
+  </si>
+  <si>
     <t>Papa Coriolis</t>
   </si>
   <si>
@@ -163,24 +172,36 @@
     <t>18:09:06</t>
   </si>
   <si>
+    <t>18:09:00</t>
+  </si>
+  <si>
     <t>18:27:57</t>
   </si>
   <si>
     <t>18:27:49</t>
   </si>
   <si>
+    <t>18:27:00</t>
+  </si>
+  <si>
     <t>18:47:09</t>
   </si>
   <si>
     <t>18:47:01</t>
   </si>
   <si>
+    <t>18:47:00</t>
+  </si>
+  <si>
     <t>19:07:10</t>
   </si>
   <si>
     <t>19:07:09</t>
   </si>
   <si>
+    <t>19:07:00</t>
+  </si>
+  <si>
     <t>Baby Coriolis</t>
   </si>
   <si>
@@ -190,6 +211,9 @@
     <t>19:27:51</t>
   </si>
   <si>
+    <t>19:27:00</t>
+  </si>
+  <si>
     <t>19:49:00</t>
   </si>
   <si>
@@ -202,88 +226,136 @@
     <t>20:10:26</t>
   </si>
   <si>
+    <t>20:10:00</t>
+  </si>
+  <si>
     <t>20:29:58</t>
   </si>
   <si>
     <t>20:29:47</t>
   </si>
   <si>
+    <t>20:29:00</t>
+  </si>
+  <si>
     <t>20:46:41</t>
   </si>
   <si>
+    <t>20:46:00</t>
+  </si>
+  <si>
     <t>16:25:02</t>
   </si>
   <si>
     <t>16:25:01</t>
   </si>
   <si>
+    <t>16:25:00</t>
+  </si>
+  <si>
     <t>16:50:52</t>
   </si>
   <si>
     <t>16:50:54</t>
   </si>
   <si>
+    <t>16:50:00</t>
+  </si>
+  <si>
     <t>17:17:02</t>
   </si>
   <si>
+    <t>17:17:00</t>
+  </si>
+  <si>
     <t>17:42:47</t>
   </si>
   <si>
     <t>17:42:41</t>
   </si>
   <si>
+    <t>17:43:00</t>
+  </si>
+  <si>
     <t>18:07:14</t>
   </si>
   <si>
     <t>18:07:05</t>
   </si>
   <si>
+    <t>18:07:00</t>
+  </si>
+  <si>
     <t>18:31:01</t>
   </si>
   <si>
     <t>18:30:51</t>
   </si>
   <si>
+    <t>18:31:00</t>
+  </si>
+  <si>
     <t>18:54:09</t>
   </si>
   <si>
     <t>18:54:05</t>
   </si>
   <si>
+    <t>18:54:00</t>
+  </si>
+  <si>
     <t>19:16:43</t>
   </si>
   <si>
     <t>19:16:34</t>
   </si>
   <si>
+    <t>19:17:00</t>
+  </si>
+  <si>
     <t>19:38:38</t>
   </si>
   <si>
     <t>19:38:31</t>
   </si>
   <si>
+    <t>19:38:00</t>
+  </si>
+  <si>
     <t>19:59:57</t>
   </si>
   <si>
     <t>19:59:55</t>
   </si>
   <si>
+    <t>20:00:00</t>
+  </si>
+  <si>
     <t>20:21:33</t>
   </si>
   <si>
     <t>20:19:49</t>
   </si>
   <si>
+    <t>20:21:00</t>
+  </si>
+  <si>
     <t>20:42:37</t>
   </si>
   <si>
     <t>20:42:28</t>
   </si>
   <si>
+    <t>20:41:00</t>
+  </si>
+  <si>
     <t>21:02:19</t>
   </si>
   <si>
     <t>21:02:17</t>
+  </si>
+  <si>
+    <t>21:02:00</t>
   </si>
 </sst>
 </file>
@@ -653,13 +725,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G27"/>
+    <sheetView tabSelected="1" topLeftCell="R4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE18" sqref="AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
@@ -825,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB2" t="s">
         <v>36</v>
@@ -856,6 +934,9 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
       <c r="E3">
         <v>2</v>
       </c>
@@ -886,40 +967,64 @@
       <c r="N3">
         <v>217.090335483871</v>
       </c>
+      <c r="O3">
+        <v>217.0276258064516</v>
+      </c>
+      <c r="P3">
+        <v>216.84818360655731</v>
+      </c>
+      <c r="Q3">
+        <v>216.76505934065929</v>
+      </c>
       <c r="R3">
-        <v>201.86334047225799</v>
+        <v>191.0241661935483</v>
       </c>
       <c r="S3">
-        <v>201.86334047225799</v>
+        <v>191.0241661935483</v>
       </c>
       <c r="T3">
-        <v>201.86334047225799</v>
+        <v>191.0241661935483</v>
       </c>
       <c r="U3">
-        <v>201.87953931096769</v>
+        <v>191.03949522580641</v>
       </c>
       <c r="V3">
-        <v>201.87953931096769</v>
+        <v>191.03949522580641</v>
       </c>
       <c r="W3">
-        <v>201.87953931096769</v>
+        <v>191.03949522580641</v>
+      </c>
+      <c r="X3">
+        <v>190.9843107096774</v>
+      </c>
+      <c r="Y3">
+        <v>190.82640157377051</v>
+      </c>
+      <c r="Z3">
+        <v>190.75325221978031</v>
       </c>
       <c r="AA3">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC3">
         <v>0</v>
       </c>
       <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
         <v>0</v>
       </c>
       <c r="AF3">
         <v>1</v>
       </c>
       <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
         <v>1</v>
       </c>
       <c r="AI3">
@@ -931,10 +1036,13 @@
         <v>44859</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -966,29 +1074,47 @@
       <c r="N4">
         <v>102.4971096774194</v>
       </c>
+      <c r="O4">
+        <v>102.7320387096774</v>
+      </c>
+      <c r="P4">
+        <v>102.7557442622951</v>
+      </c>
+      <c r="Q4">
+        <v>102.7890197802198</v>
+      </c>
       <c r="R4">
-        <v>95.300359943225757</v>
+        <v>90.183149419354862</v>
       </c>
       <c r="S4">
-        <v>95.300359943225757</v>
+        <v>90.183149419354862</v>
       </c>
       <c r="T4">
-        <v>95.300359943225757</v>
+        <v>90.183149419354862</v>
       </c>
       <c r="U4">
-        <v>95.315478859354769</v>
+        <v>90.197456516129066</v>
       </c>
       <c r="V4">
-        <v>95.315478859354769</v>
+        <v>90.197456516129066</v>
       </c>
       <c r="W4">
-        <v>95.315478859354769</v>
+        <v>90.197456516129066</v>
+      </c>
+      <c r="X4">
+        <v>90.404194064516133</v>
+      </c>
+      <c r="Y4">
+        <v>90.425054950819685</v>
+      </c>
+      <c r="Z4">
+        <v>90.454337406593424</v>
       </c>
       <c r="AA4">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC4">
         <v>0</v>
@@ -996,10 +1122,16 @@
       <c r="AD4">
         <v>0</v>
       </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
       <c r="AF4">
         <v>0</v>
       </c>
       <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
         <v>0</v>
       </c>
       <c r="AI4">
@@ -1011,10 +1143,13 @@
         <v>44859</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1046,29 +1181,47 @@
       <c r="N5">
         <v>1041.336</v>
       </c>
+      <c r="O5">
+        <v>1050.192</v>
+      </c>
+      <c r="P5">
+        <v>1042.1598688524591</v>
+      </c>
+      <c r="Q5">
+        <v>1042.268439560439</v>
+      </c>
       <c r="R5">
-        <v>968.34821938064488</v>
+        <v>916.35217548387106</v>
       </c>
       <c r="S5">
-        <v>968.34821938064488</v>
+        <v>916.35217548387106</v>
       </c>
       <c r="T5">
-        <v>968.34821938064488</v>
+        <v>916.35217548387106</v>
       </c>
       <c r="U5">
-        <v>968.37305759999958</v>
+        <v>916.37568000000022</v>
       </c>
       <c r="V5">
-        <v>968.37305759999958</v>
+        <v>916.37568000000022</v>
       </c>
       <c r="W5">
-        <v>968.37305759999958</v>
+        <v>916.37568000000022</v>
+      </c>
+      <c r="X5">
+        <v>924.16896000000008</v>
+      </c>
+      <c r="Y5">
+        <v>917.10068459016395</v>
+      </c>
+      <c r="Z5">
+        <v>917.19622681318674</v>
       </c>
       <c r="AA5">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC5">
         <v>1</v>
@@ -1076,10 +1229,16 @@
       <c r="AD5">
         <v>1</v>
       </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
       <c r="AF5">
         <v>1</v>
       </c>
       <c r="AG5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
         <v>1</v>
       </c>
       <c r="AI5">
@@ -1091,10 +1250,13 @@
         <v>44859</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -1126,29 +1288,47 @@
       <c r="N6">
         <v>1040.3036129032259</v>
       </c>
+      <c r="O6">
+        <v>1037.837032258064</v>
+      </c>
+      <c r="P6">
+        <v>1031.668524590164</v>
+      </c>
+      <c r="Q6">
+        <v>1033.024351648352</v>
+      </c>
       <c r="R6">
-        <v>966.63870193548348</v>
+        <v>914.7344516129034</v>
       </c>
       <c r="S6">
-        <v>966.63870193548348</v>
+        <v>914.7344516129034</v>
       </c>
       <c r="T6">
-        <v>966.63870193548348</v>
+        <v>914.7344516129034</v>
       </c>
       <c r="U6">
-        <v>967.41300642580586</v>
+        <v>915.46717935483889</v>
       </c>
       <c r="V6">
-        <v>967.41300642580586</v>
+        <v>915.46717935483889</v>
       </c>
       <c r="W6">
-        <v>967.41300642580586</v>
+        <v>915.46717935483889</v>
+      </c>
+      <c r="X6">
+        <v>913.29658838709668</v>
+      </c>
+      <c r="Y6">
+        <v>907.86830163934417</v>
+      </c>
+      <c r="Z6">
+        <v>909.06142945054944</v>
       </c>
       <c r="AA6">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -1156,10 +1336,16 @@
       <c r="AD6">
         <v>0</v>
       </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
       <c r="AF6">
         <v>0</v>
       </c>
       <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
         <v>0</v>
       </c>
       <c r="AI6">
@@ -1171,10 +1357,13 @@
         <v>44859</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -1206,6 +1395,15 @@
       <c r="N7">
         <v>0</v>
       </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
       <c r="R7">
         <v>0</v>
       </c>
@@ -1224,8 +1422,17 @@
       <c r="W7">
         <v>0</v>
       </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
       <c r="AA7">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB7" t="s">
         <v>36</v>
@@ -1236,10 +1443,16 @@
       <c r="AD7">
         <v>1</v>
       </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
       <c r="AF7">
         <v>1</v>
       </c>
       <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
         <v>1</v>
       </c>
       <c r="AI7">
@@ -1251,10 +1464,13 @@
         <v>44859</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -1286,29 +1502,47 @@
       <c r="N8">
         <v>493.09548387096783</v>
       </c>
+      <c r="O8">
+        <v>493.18606451612902</v>
+      </c>
+      <c r="P8">
+        <v>492.88721311475422</v>
+      </c>
+      <c r="Q8">
+        <v>492.86413186813189</v>
+      </c>
       <c r="R8">
-        <v>457.81697922580628</v>
+        <v>433.23421935483867</v>
       </c>
       <c r="S8">
-        <v>457.81697922580628</v>
+        <v>433.23421935483867</v>
       </c>
       <c r="T8">
-        <v>457.81697922580628</v>
+        <v>433.23421935483867</v>
       </c>
       <c r="U8">
-        <v>458.54592696774182</v>
+        <v>433.9240258064516</v>
       </c>
       <c r="V8">
-        <v>458.54592696774182</v>
+        <v>433.9240258064516</v>
       </c>
       <c r="W8">
-        <v>458.54592696774182</v>
+        <v>433.9240258064516</v>
+      </c>
+      <c r="X8">
+        <v>434.00373677419361</v>
+      </c>
+      <c r="Y8">
+        <v>433.74074754098359</v>
+      </c>
+      <c r="Z8">
+        <v>433.720436043956</v>
       </c>
       <c r="AA8">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC8">
         <v>0</v>
@@ -1316,10 +1550,16 @@
       <c r="AD8">
         <v>0</v>
       </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
       <c r="AF8">
         <v>0</v>
       </c>
       <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
         <v>0</v>
       </c>
       <c r="AI8">
@@ -1331,10 +1571,13 @@
         <v>44859</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1366,29 +1609,47 @@
       <c r="N9">
         <v>25.675258064516129</v>
       </c>
+      <c r="O9">
+        <v>25.673829677419359</v>
+      </c>
+      <c r="P9">
+        <v>25.69508262295081</v>
+      </c>
+      <c r="Q9">
+        <v>25.709312967032979</v>
+      </c>
       <c r="R9">
-        <v>23.875079602064499</v>
+        <v>22.5930927483871</v>
       </c>
       <c r="S9">
-        <v>23.875079602064499</v>
+        <v>22.5930927483871</v>
       </c>
       <c r="T9">
-        <v>23.875079602064499</v>
+        <v>22.5930927483871</v>
       </c>
       <c r="U9">
-        <v>23.876278316129021</v>
+        <v>22.594227096774201</v>
       </c>
       <c r="V9">
-        <v>23.876278316129021</v>
+        <v>22.594227096774201</v>
       </c>
       <c r="W9">
-        <v>23.876278316129021</v>
+        <v>22.594227096774201</v>
+      </c>
+      <c r="X9">
+        <v>22.592970116129031</v>
+      </c>
+      <c r="Y9">
+        <v>22.611672708196721</v>
+      </c>
+      <c r="Z9">
+        <v>22.62419541098901</v>
       </c>
       <c r="AA9">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB9" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -1396,10 +1657,16 @@
       <c r="AD9">
         <v>0</v>
       </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
       <c r="AF9">
         <v>0</v>
       </c>
       <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
         <v>0</v>
       </c>
       <c r="AI9">
@@ -1411,10 +1678,13 @@
         <v>44859</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
       </c>
       <c r="E10">
         <v>9</v>
@@ -1446,29 +1716,47 @@
       <c r="N10">
         <v>667.92193548387093</v>
       </c>
+      <c r="O10">
+        <v>667.88709677419354</v>
+      </c>
+      <c r="P10">
+        <v>668.34649180327881</v>
+      </c>
+      <c r="Q10">
+        <v>667.82452747252751</v>
+      </c>
       <c r="R10">
-        <v>621.35181545806438</v>
+        <v>587.98795354838717</v>
       </c>
       <c r="S10">
-        <v>621.35181545806438</v>
+        <v>587.98795354838717</v>
       </c>
       <c r="T10">
-        <v>621.35181545806438</v>
+        <v>587.98795354838717</v>
       </c>
       <c r="U10">
-        <v>621.12287187096763</v>
+        <v>587.77130322580649</v>
       </c>
       <c r="V10">
-        <v>621.12287187096763</v>
+        <v>587.77130322580649</v>
       </c>
       <c r="W10">
-        <v>621.12287187096763</v>
+        <v>587.77130322580649</v>
+      </c>
+      <c r="X10">
+        <v>587.74064516129022</v>
+      </c>
+      <c r="Y10">
+        <v>588.14491278688524</v>
+      </c>
+      <c r="Z10">
+        <v>587.68558417582415</v>
       </c>
       <c r="AA10">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC10">
         <v>0</v>
@@ -1476,10 +1764,16 @@
       <c r="AD10">
         <v>0</v>
       </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
       <c r="AF10">
         <v>0</v>
       </c>
       <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
         <v>0</v>
       </c>
       <c r="AI10">
@@ -1491,10 +1785,10 @@
         <v>44859</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -1524,28 +1818,28 @@
         <v>363.82099354838709</v>
       </c>
       <c r="R11">
-        <v>338.7072421703225</v>
+        <v>320.52015174193542</v>
       </c>
       <c r="S11">
-        <v>338.7072421703225</v>
+        <v>320.52015174193542</v>
       </c>
       <c r="T11">
-        <v>338.7072421703225</v>
+        <v>320.52015174193542</v>
       </c>
       <c r="U11">
-        <v>338.32926926709672</v>
+        <v>320.16247432258058</v>
       </c>
       <c r="V11">
-        <v>338.32926926709672</v>
+        <v>320.16247432258058</v>
       </c>
       <c r="W11">
-        <v>338.32926926709672</v>
+        <v>320.16247432258058</v>
       </c>
       <c r="AA11">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC11">
         <v>0</v>
@@ -1568,10 +1862,13 @@
         <v>44859</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
       </c>
       <c r="E12">
         <v>11</v>
@@ -1603,29 +1900,47 @@
       <c r="N12">
         <v>149.5282064516129</v>
       </c>
+      <c r="O12">
+        <v>149.53517419354839</v>
+      </c>
+      <c r="P12">
+        <v>149.56241311475409</v>
+      </c>
+      <c r="Q12">
+        <v>149.5834417582418</v>
+      </c>
       <c r="R12">
-        <v>139.02577727999989</v>
+        <v>131.56070399999999</v>
       </c>
       <c r="S12">
-        <v>139.02577727999989</v>
+        <v>131.56070399999999</v>
       </c>
       <c r="T12">
-        <v>139.02577727999989</v>
+        <v>131.56070399999999</v>
       </c>
       <c r="U12">
-        <v>139.05126345290321</v>
+        <v>131.5848216774194</v>
       </c>
       <c r="V12">
-        <v>139.05126345290321</v>
+        <v>131.5848216774194</v>
       </c>
       <c r="W12">
-        <v>139.05126345290321</v>
+        <v>131.5848216774194</v>
+      </c>
+      <c r="X12">
+        <v>131.5909532903226</v>
+      </c>
+      <c r="Y12">
+        <v>131.6149235409836</v>
+      </c>
+      <c r="Z12">
+        <v>131.63342874725271</v>
       </c>
       <c r="AA12">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -1633,10 +1948,16 @@
       <c r="AD12">
         <v>0</v>
       </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
       <c r="AF12">
         <v>0</v>
       </c>
       <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
         <v>0</v>
       </c>
       <c r="AI12">
@@ -1648,10 +1969,13 @@
         <v>44859</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
       </c>
       <c r="E13">
         <v>12</v>
@@ -1683,40 +2007,64 @@
       <c r="N13">
         <v>78.507638709677408</v>
       </c>
+      <c r="O13">
+        <v>78.672774193548378</v>
+      </c>
+      <c r="P13">
+        <v>78.73229508196718</v>
+      </c>
+      <c r="Q13">
+        <v>78.754312087912069</v>
+      </c>
       <c r="R13">
-        <v>72.977712247741906</v>
+        <v>69.059129806451608</v>
       </c>
       <c r="S13">
-        <v>72.977712247741906</v>
+        <v>69.059129806451608</v>
       </c>
       <c r="T13">
-        <v>72.977712247741906</v>
+        <v>69.059129806451608</v>
       </c>
       <c r="U13">
-        <v>73.0068701574193</v>
+        <v>69.086722064516138</v>
       </c>
       <c r="V13">
-        <v>73.0068701574193</v>
+        <v>69.086722064516138</v>
       </c>
       <c r="W13">
-        <v>73.0068701574193</v>
+        <v>69.086722064516138</v>
+      </c>
+      <c r="X13">
+        <v>69.232041290322599</v>
+      </c>
+      <c r="Y13">
+        <v>69.28441967213115</v>
+      </c>
+      <c r="Z13">
+        <v>69.303794637362643</v>
       </c>
       <c r="AA13">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC13">
         <v>0</v>
       </c>
       <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
         <v>0</v>
       </c>
       <c r="AF13">
         <v>1</v>
       </c>
       <c r="AG13">
+        <v>1</v>
+      </c>
+      <c r="AH13">
         <v>1</v>
       </c>
       <c r="AI13">
@@ -1728,10 +2076,13 @@
         <v>44859</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
       </c>
       <c r="E14">
         <v>13</v>
@@ -1763,29 +2114,47 @@
       <c r="N14">
         <v>66.313175806451611</v>
       </c>
+      <c r="O14">
+        <v>66.31533870967742</v>
+      </c>
+      <c r="P14">
+        <v>66.338358196721302</v>
+      </c>
+      <c r="Q14">
+        <v>66.363923076923072</v>
+      </c>
       <c r="R14">
-        <v>61.666832621612883</v>
+        <v>58.355594709677433</v>
       </c>
       <c r="S14">
-        <v>61.666832621612883</v>
+        <v>58.355594709677433</v>
       </c>
       <c r="T14">
-        <v>61.666832621612883</v>
+        <v>58.355594709677433</v>
       </c>
       <c r="U14">
-        <v>61.666832621612883</v>
+        <v>58.355594709677433</v>
       </c>
       <c r="V14">
-        <v>61.666832621612883</v>
+        <v>58.355594709677433</v>
       </c>
       <c r="W14">
-        <v>61.666832621612883</v>
+        <v>58.355594709677433</v>
+      </c>
+      <c r="X14">
+        <v>58.357498064516129</v>
+      </c>
+      <c r="Y14">
+        <v>58.377755213114753</v>
+      </c>
+      <c r="Z14">
+        <v>58.400252307692313</v>
       </c>
       <c r="AA14">
-        <v>0.92993333333333295</v>
+        <v>0.88</v>
       </c>
       <c r="AB14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC14">
         <v>0</v>
@@ -1793,10 +2162,16 @@
       <c r="AD14">
         <v>0</v>
       </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
       <c r="AF14">
         <v>0</v>
       </c>
       <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
         <v>0</v>
       </c>
       <c r="AI14">
@@ -1808,10 +2183,13 @@
         <v>44863</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
       </c>
       <c r="E15">
         <v>14</v>
@@ -1843,6 +2221,15 @@
       <c r="N15">
         <v>0</v>
       </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
       <c r="R15">
         <v>0</v>
       </c>
@@ -1861,8 +2248,17 @@
       <c r="W15">
         <v>0</v>
       </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
       <c r="AA15">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB15" t="s">
         <v>36</v>
@@ -1873,10 +2269,16 @@
       <c r="AD15">
         <v>0</v>
       </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
       <c r="AF15">
         <v>0</v>
       </c>
       <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
         <v>0</v>
       </c>
       <c r="AI15">
@@ -1888,10 +2290,13 @@
         <v>44863</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
       </c>
       <c r="E16">
         <v>15</v>
@@ -1923,29 +2328,47 @@
       <c r="N16">
         <v>356.91329032258068</v>
       </c>
+      <c r="O16">
+        <v>356.5243741935484</v>
+      </c>
+      <c r="P16">
+        <v>356.53296393442622</v>
+      </c>
+      <c r="Q16">
+        <v>356.51990769230758</v>
+      </c>
       <c r="R16">
-        <v>342.60120885677429</v>
+        <v>331.94102400000003</v>
       </c>
       <c r="S16">
-        <v>342.60120885677429</v>
+        <v>331.94102400000003</v>
       </c>
       <c r="T16">
-        <v>342.60120885677429</v>
+        <v>331.94102400000003</v>
       </c>
       <c r="U16">
-        <v>342.58917027096788</v>
+        <v>331.92935999999997</v>
       </c>
       <c r="V16">
-        <v>342.58917027096788</v>
+        <v>331.92935999999997</v>
       </c>
       <c r="W16">
-        <v>342.58917027096788</v>
+        <v>331.92935999999997</v>
+      </c>
+      <c r="X16">
+        <v>331.56766800000003</v>
+      </c>
+      <c r="Y16">
+        <v>331.57565645901639</v>
+      </c>
+      <c r="Z16">
+        <v>331.56351415384609</v>
       </c>
       <c r="AA16">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC16">
         <v>0</v>
@@ -1953,10 +2376,16 @@
       <c r="AD16">
         <v>0</v>
       </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
       <c r="AF16">
         <v>0</v>
       </c>
       <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16">
         <v>0</v>
       </c>
       <c r="AI16">
@@ -1968,10 +2397,13 @@
         <v>44863</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="D17" t="s">
+        <v>81</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -2003,29 +2435,47 @@
       <c r="N17">
         <v>704.6372903225805</v>
       </c>
+      <c r="O17">
+        <v>704.59780645161288</v>
+      </c>
+      <c r="P17">
+        <v>704.57960655737713</v>
+      </c>
+      <c r="Q17">
+        <v>704.23556043956046</v>
+      </c>
       <c r="R17">
-        <v>676.35784707096809</v>
+        <v>655.31267999999989</v>
       </c>
       <c r="S17">
-        <v>676.35784707096809</v>
+        <v>655.31267999999989</v>
       </c>
       <c r="T17">
-        <v>676.35784707096809</v>
+        <v>655.31267999999989</v>
       </c>
       <c r="U17">
-        <v>676.35784707096809</v>
+        <v>655.31267999999989</v>
       </c>
       <c r="V17">
-        <v>676.35784707096809</v>
+        <v>655.31267999999989</v>
       </c>
       <c r="W17">
-        <v>676.35784707096809</v>
+        <v>655.31267999999989</v>
+      </c>
+      <c r="X17">
+        <v>655.27595999999983</v>
+      </c>
+      <c r="Y17">
+        <v>655.25903409836076</v>
+      </c>
+      <c r="Z17">
+        <v>654.93907120879135</v>
       </c>
       <c r="AA17">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC17">
         <v>0</v>
@@ -2033,10 +2483,16 @@
       <c r="AD17">
         <v>0</v>
       </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
       <c r="AF17">
         <v>0</v>
       </c>
       <c r="AG17">
+        <v>0</v>
+      </c>
+      <c r="AH17">
         <v>0</v>
       </c>
       <c r="AI17">
@@ -2048,10 +2504,13 @@
         <v>44863</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>84</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -2083,29 +2542,47 @@
       <c r="N18">
         <v>425.68141935483868</v>
       </c>
+      <c r="O18">
+        <v>425.84748387096772</v>
+      </c>
+      <c r="P18">
+        <v>425.77259016393452</v>
+      </c>
+      <c r="Q18">
+        <v>425.42268131868133</v>
+      </c>
       <c r="R18">
-        <v>408.69326787096787</v>
+        <v>395.97660000000008</v>
       </c>
       <c r="S18">
-        <v>408.69326787096787</v>
+        <v>395.97660000000008</v>
       </c>
       <c r="T18">
-        <v>408.69326787096787</v>
+        <v>395.97660000000008</v>
       </c>
       <c r="U18">
-        <v>408.59740505806462</v>
+        <v>395.8837200000001</v>
       </c>
       <c r="V18">
-        <v>408.59740505806462</v>
+        <v>395.8837200000001</v>
       </c>
       <c r="W18">
-        <v>408.59740505806462</v>
+        <v>395.8837200000001</v>
+      </c>
+      <c r="X18">
+        <v>396.03815999999989</v>
+      </c>
+      <c r="Y18">
+        <v>395.96850885245902</v>
+      </c>
+      <c r="Z18">
+        <v>395.64309362637368</v>
       </c>
       <c r="AA18">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB18" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC18">
         <v>0</v>
@@ -2113,11 +2590,17 @@
       <c r="AD18">
         <v>0</v>
       </c>
+      <c r="AE18">
+        <v>1</v>
+      </c>
       <c r="AF18">
         <v>0</v>
       </c>
       <c r="AG18">
         <v>0</v>
+      </c>
+      <c r="AH18">
+        <v>1</v>
       </c>
       <c r="AI18">
         <v>45048.954918032781</v>
@@ -2128,10 +2611,13 @@
         <v>44863</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>86</v>
+      </c>
+      <c r="D19" t="s">
+        <v>87</v>
       </c>
       <c r="E19">
         <v>18</v>
@@ -2163,29 +2649,47 @@
       <c r="N19">
         <v>35.239169032258069</v>
       </c>
+      <c r="O19">
+        <v>35.243489032258061</v>
+      </c>
+      <c r="P19">
+        <v>35.261020327868849</v>
+      </c>
+      <c r="Q19">
+        <v>35.280178021978017</v>
+      </c>
       <c r="R19">
-        <v>33.821236405161287</v>
+        <v>32.768873999999997</v>
       </c>
       <c r="S19">
-        <v>33.821236405161287</v>
+        <v>32.768873999999997</v>
       </c>
       <c r="T19">
-        <v>33.821236405161287</v>
+        <v>32.768873999999997</v>
       </c>
       <c r="U19">
-        <v>33.824903715096781</v>
+        <v>32.772427200000003</v>
       </c>
       <c r="V19">
-        <v>33.824903715096781</v>
+        <v>32.772427200000003</v>
       </c>
       <c r="W19">
-        <v>33.824903715096781</v>
+        <v>32.772427200000003</v>
+      </c>
+      <c r="X19">
+        <v>32.7764448</v>
+      </c>
+      <c r="Y19">
+        <v>32.792748904918042</v>
+      </c>
+      <c r="Z19">
+        <v>32.810565560439557</v>
       </c>
       <c r="AA19">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB19" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="AC19">
         <v>0</v>
@@ -2193,10 +2697,16 @@
       <c r="AD19">
         <v>0</v>
       </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
       <c r="AF19">
         <v>0</v>
       </c>
       <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AH19">
         <v>0</v>
       </c>
       <c r="AI19">
@@ -2208,10 +2718,13 @@
         <v>44863</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>89</v>
+      </c>
+      <c r="D20" t="s">
+        <v>90</v>
       </c>
       <c r="E20">
         <v>19</v>
@@ -2243,29 +2756,47 @@
       <c r="N20">
         <v>354.19494193548388</v>
       </c>
+      <c r="O20">
+        <v>354.35241290322591</v>
+      </c>
+      <c r="P20">
+        <v>354.08083278688531</v>
+      </c>
+      <c r="Q20">
+        <v>353.89420219780231</v>
+      </c>
       <c r="R20">
-        <v>340.12560744774203</v>
+        <v>329.54245200000003</v>
       </c>
       <c r="S20">
-        <v>340.12560744774203</v>
+        <v>329.54245200000003</v>
       </c>
       <c r="T20">
-        <v>340.12560744774203</v>
+        <v>329.54245200000003</v>
       </c>
       <c r="U20">
-        <v>339.97991826580648</v>
+        <v>329.401296</v>
       </c>
       <c r="V20">
-        <v>339.97991826580648</v>
+        <v>329.401296</v>
       </c>
       <c r="W20">
-        <v>339.97991826580648</v>
+        <v>329.401296</v>
+      </c>
+      <c r="X20">
+        <v>329.54774400000002</v>
+      </c>
+      <c r="Y20">
+        <v>329.29517449180321</v>
+      </c>
+      <c r="Z20">
+        <v>329.12160804395597</v>
       </c>
       <c r="AA20">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC20">
         <v>0</v>
@@ -2273,10 +2804,16 @@
       <c r="AD20">
         <v>0</v>
       </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
       <c r="AF20">
         <v>0</v>
       </c>
       <c r="AG20">
+        <v>0</v>
+      </c>
+      <c r="AH20">
         <v>0</v>
       </c>
       <c r="AI20">
@@ -2288,10 +2825,13 @@
         <v>44863</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>93</v>
       </c>
       <c r="E21">
         <v>20</v>
@@ -2323,29 +2863,47 @@
       <c r="N21">
         <v>858.793935483871</v>
       </c>
+      <c r="O21">
+        <v>860.14103225806457</v>
+      </c>
+      <c r="P21">
+        <v>858.64603278688526</v>
+      </c>
+      <c r="Q21">
+        <v>859.29547252747238</v>
+      </c>
       <c r="R21">
-        <v>822.50850812903241</v>
+        <v>796.91579999999999</v>
       </c>
       <c r="S21">
-        <v>822.50850812903241</v>
+        <v>796.91579999999999</v>
       </c>
       <c r="T21">
-        <v>822.50850812903241</v>
+        <v>796.91579999999999</v>
       </c>
       <c r="U21">
-        <v>824.32767220645189</v>
+        <v>798.67836000000011</v>
       </c>
       <c r="V21">
-        <v>824.32767220645189</v>
+        <v>798.67836000000011</v>
       </c>
       <c r="W21">
-        <v>824.32767220645189</v>
+        <v>798.67836000000011</v>
+      </c>
+      <c r="X21">
+        <v>799.93116000000009</v>
+      </c>
+      <c r="Y21">
+        <v>798.54081049180331</v>
+      </c>
+      <c r="Z21">
+        <v>799.1447894505493</v>
       </c>
       <c r="AA21">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB21" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC21">
         <v>0</v>
@@ -2353,10 +2911,16 @@
       <c r="AD21">
         <v>0</v>
       </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
       <c r="AF21">
         <v>0</v>
       </c>
       <c r="AG21">
+        <v>0</v>
+      </c>
+      <c r="AH21">
         <v>0</v>
       </c>
       <c r="AI21">
@@ -2368,10 +2932,13 @@
         <v>44863</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>95</v>
+      </c>
+      <c r="D22" t="s">
+        <v>96</v>
       </c>
       <c r="E22">
         <v>21</v>
@@ -2403,29 +2970,47 @@
       <c r="N22">
         <v>1120.091225806452</v>
       </c>
+      <c r="O22">
+        <v>1110.8763870967739</v>
+      </c>
+      <c r="P22">
+        <v>1113.8736393442621</v>
+      </c>
+      <c r="Q22">
+        <v>1114.186153846154</v>
+      </c>
       <c r="R22">
-        <v>1070.648284645162</v>
+        <v>1037.3345999999999</v>
       </c>
       <c r="S22">
-        <v>1070.648284645162</v>
+        <v>1037.3345999999999</v>
       </c>
       <c r="T22">
-        <v>1070.648284645162</v>
+        <v>1037.3345999999999</v>
       </c>
       <c r="U22">
-        <v>1075.1382312774199</v>
+        <v>1041.6848399999999</v>
       </c>
       <c r="V22">
-        <v>1075.1382312774199</v>
+        <v>1041.6848399999999</v>
       </c>
       <c r="W22">
-        <v>1075.1382312774199</v>
+        <v>1041.6848399999999</v>
+      </c>
+      <c r="X22">
+        <v>1033.1150399999999</v>
+      </c>
+      <c r="Y22">
+        <v>1035.902484590164</v>
+      </c>
+      <c r="Z22">
+        <v>1036.193123076923</v>
       </c>
       <c r="AA22">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB22" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC22">
         <v>0</v>
@@ -2433,10 +3018,16 @@
       <c r="AD22">
         <v>0</v>
       </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
       <c r="AF22">
         <v>0</v>
       </c>
       <c r="AG22">
+        <v>0</v>
+      </c>
+      <c r="AH22">
         <v>0</v>
       </c>
       <c r="AI22">
@@ -2448,10 +3039,13 @@
         <v>44863</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>99</v>
       </c>
       <c r="E23">
         <v>22</v>
@@ -2483,29 +3077,47 @@
       <c r="N23">
         <v>1360.9358709677419</v>
       </c>
+      <c r="O23">
+        <v>1352.680258064516</v>
+      </c>
+      <c r="P23">
+        <v>1354.059737704918</v>
+      </c>
+      <c r="Q23">
+        <v>1357.4523956043961</v>
+      </c>
       <c r="R23">
-        <v>1299.8941695483879</v>
+        <v>1259.4474</v>
       </c>
       <c r="S23">
-        <v>1299.8941695483879</v>
+        <v>1259.4474</v>
       </c>
       <c r="T23">
-        <v>1299.8941695483879</v>
+        <v>1259.4474</v>
       </c>
       <c r="U23">
-        <v>1306.316978012904</v>
+        <v>1265.6703600000001</v>
       </c>
       <c r="V23">
-        <v>1306.316978012904</v>
+        <v>1265.6703600000001</v>
       </c>
       <c r="W23">
-        <v>1306.316978012904</v>
+        <v>1265.6703600000001</v>
+      </c>
+      <c r="X23">
+        <v>1257.9926399999999</v>
+      </c>
+      <c r="Y23">
+        <v>1259.2755560655739</v>
+      </c>
+      <c r="Z23">
+        <v>1262.4307279120881</v>
       </c>
       <c r="AA23">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC23">
         <v>0</v>
@@ -2513,11 +3125,17 @@
       <c r="AD23">
         <v>0</v>
       </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
       <c r="AF23">
         <v>0</v>
       </c>
       <c r="AG23">
         <v>0</v>
+      </c>
+      <c r="AH23">
+        <v>1</v>
       </c>
       <c r="AI23">
         <v>46025</v>
@@ -2528,10 +3146,13 @@
         <v>44863</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>101</v>
+      </c>
+      <c r="D24" t="s">
+        <v>102</v>
       </c>
       <c r="E24">
         <v>23</v>
@@ -2563,29 +3184,47 @@
       <c r="N24">
         <v>613.4330322580646</v>
       </c>
+      <c r="O24">
+        <v>613.70012903225802</v>
+      </c>
+      <c r="P24">
+        <v>613.96701639344258</v>
+      </c>
+      <c r="Q24">
+        <v>614.1287472527473</v>
+      </c>
       <c r="R24">
-        <v>589.04354477419383</v>
+        <v>570.7152000000001</v>
       </c>
       <c r="S24">
-        <v>589.04354477419383</v>
+        <v>570.7152000000001</v>
       </c>
       <c r="T24">
-        <v>589.04354477419383</v>
+        <v>570.7152000000001</v>
       </c>
       <c r="U24">
-        <v>588.81391989677434</v>
+        <v>570.49271999999996</v>
       </c>
       <c r="V24">
-        <v>588.81391989677434</v>
+        <v>570.49271999999996</v>
       </c>
       <c r="W24">
-        <v>588.81391989677434</v>
+        <v>570.49271999999996</v>
+      </c>
+      <c r="X24">
+        <v>570.74112000000014</v>
+      </c>
+      <c r="Y24">
+        <v>570.98932524590157</v>
+      </c>
+      <c r="Z24">
+        <v>571.1397349450549</v>
       </c>
       <c r="AA24">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB24" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC24">
         <v>0</v>
@@ -2593,10 +3232,16 @@
       <c r="AD24">
         <v>0</v>
       </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
       <c r="AF24">
         <v>0</v>
       </c>
       <c r="AG24">
+        <v>0</v>
+      </c>
+      <c r="AH24">
         <v>0</v>
       </c>
       <c r="AI24">
@@ -2608,10 +3253,13 @@
         <v>44863</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
+        <v>105</v>
       </c>
       <c r="E25">
         <v>24</v>
@@ -2643,29 +3291,47 @@
       <c r="N25">
         <v>214.20685161290319</v>
       </c>
+      <c r="O25">
+        <v>214.33900645161279</v>
+      </c>
+      <c r="P25">
+        <v>214.32275409836069</v>
+      </c>
+      <c r="Q25">
+        <v>214.31425054945061</v>
+      </c>
       <c r="R25">
-        <v>195.87481357935491</v>
+        <v>189.78008399999999</v>
       </c>
       <c r="S25">
-        <v>195.87481357935491</v>
+        <v>189.78008399999999</v>
       </c>
       <c r="T25">
-        <v>195.87481357935491</v>
+        <v>189.78008399999999</v>
       </c>
       <c r="U25">
-        <v>205.61001663483879</v>
+        <v>199.21237199999999</v>
       </c>
       <c r="V25">
-        <v>205.61001663483879</v>
+        <v>199.21237199999999</v>
       </c>
       <c r="W25">
-        <v>205.61001663483879</v>
+        <v>199.21237199999999</v>
+      </c>
+      <c r="X25">
+        <v>199.33527600000011</v>
+      </c>
+      <c r="Y25">
+        <v>199.3201613114754</v>
+      </c>
+      <c r="Z25">
+        <v>199.312253010989</v>
       </c>
       <c r="AA25">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC25">
         <v>1</v>
@@ -2673,10 +3339,16 @@
       <c r="AD25">
         <v>0</v>
       </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
       <c r="AF25">
         <v>1</v>
       </c>
       <c r="AG25">
+        <v>0</v>
+      </c>
+      <c r="AH25">
         <v>0</v>
       </c>
       <c r="AI25">
@@ -2688,10 +3360,13 @@
         <v>44863</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>107</v>
+      </c>
+      <c r="D26" t="s">
+        <v>108</v>
       </c>
       <c r="E26">
         <v>25</v>
@@ -2723,29 +3398,47 @@
       <c r="N26">
         <v>518.1863225806452</v>
       </c>
+      <c r="O26">
+        <v>519.09096774193551</v>
+      </c>
+      <c r="P26">
+        <v>519.28701639344263</v>
+      </c>
+      <c r="Q26">
+        <v>519.39969230769225</v>
+      </c>
       <c r="R26">
-        <v>497.00298286451618</v>
+        <v>481.53852000000001</v>
       </c>
       <c r="S26">
-        <v>497.00298286451618</v>
+        <v>481.53852000000001</v>
       </c>
       <c r="T26">
-        <v>497.00298286451618</v>
+        <v>481.53852000000001</v>
       </c>
       <c r="U26">
-        <v>497.38977816774212</v>
+        <v>481.91327999999999</v>
       </c>
       <c r="V26">
-        <v>497.38977816774212</v>
+        <v>481.91327999999999</v>
       </c>
       <c r="W26">
-        <v>497.38977816774212</v>
+        <v>481.91327999999999</v>
+      </c>
+      <c r="X26">
+        <v>482.75459999999998</v>
+      </c>
+      <c r="Y26">
+        <v>482.93692524590159</v>
+      </c>
+      <c r="Z26">
+        <v>483.04171384615393</v>
       </c>
       <c r="AA26">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB26" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC26">
         <v>1</v>
@@ -2768,10 +3461,13 @@
         <v>44863</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>110</v>
+      </c>
+      <c r="D27" t="s">
+        <v>111</v>
       </c>
       <c r="E27">
         <v>26</v>
@@ -2803,29 +3499,47 @@
       <c r="N27">
         <v>177.0741435483871</v>
       </c>
+      <c r="O27">
+        <v>177.09869032258061</v>
+      </c>
+      <c r="P27">
+        <v>177.13447377049181</v>
+      </c>
+      <c r="Q27">
+        <v>177.11081703296699</v>
+      </c>
       <c r="R27">
-        <v>169.97357328000001</v>
+        <v>164.68477200000001</v>
       </c>
       <c r="S27">
-        <v>169.97357328000001</v>
+        <v>164.68477200000001</v>
       </c>
       <c r="T27">
-        <v>169.97357328000001</v>
+        <v>164.68477200000001</v>
       </c>
       <c r="U27">
-        <v>169.96756792064519</v>
+        <v>164.67895350000001</v>
       </c>
       <c r="V27">
-        <v>169.96756792064519</v>
+        <v>164.67895350000001</v>
       </c>
       <c r="W27">
-        <v>169.96756792064519</v>
+        <v>164.67895350000001</v>
+      </c>
+      <c r="X27">
+        <v>164.70178200000001</v>
+      </c>
+      <c r="Y27">
+        <v>164.7350606065574</v>
+      </c>
+      <c r="Z27">
+        <v>164.7130598406593</v>
       </c>
       <c r="AA27">
-        <v>0.95986666666666698</v>
+        <v>0.93</v>
       </c>
       <c r="AB27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC27">
         <v>0</v>
@@ -2833,10 +3547,16 @@
       <c r="AD27">
         <v>0</v>
       </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
       <c r="AF27">
         <v>0</v>
       </c>
       <c r="AG27">
+        <v>0</v>
+      </c>
+      <c r="AH27">
         <v>0</v>
       </c>
       <c r="AI27">

</xml_diff>